<commit_message>
Correction des valeurs - d'altitude négative - de hauteur d'eau > 9m - de coordonnées de la station Embouchure
</commit_message>
<xml_diff>
--- a/data/station.xlsx
+++ b/data/station.xlsx
@@ -8747,10 +8747,10 @@
         </is>
       </c>
       <c r="N134">
-        <v>1.439964216</v>
+        <v>1.41282</v>
       </c>
       <c r="O134">
-        <v>43.597961996</v>
+        <v>43.609488</v>
       </c>
     </row>
   </sheetData>

</xml_diff>